<commit_message>
false_S proteins were added
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="153">
   <si>
     <t>_id</t>
   </si>
@@ -445,6 +445,45 @@
   </si>
   <si>
     <t>DUF3520 domain-containing protein (Pseudomonas anguilliseptica)</t>
+  </si>
+  <si>
+    <t>Rv2208</t>
+  </si>
+  <si>
+    <t>adenosylcobinamide-GDP ribazoletransferase (Mycobacterium tuberculosis H37Rv)</t>
+  </si>
+  <si>
+    <t>PP_1681</t>
+  </si>
+  <si>
+    <t>adenosylcobinamide-GDP ribazoletransferase (Pseudomonas putida KT2440)</t>
+  </si>
+  <si>
+    <t>RD1_RS07205</t>
+  </si>
+  <si>
+    <t>CbbQ/NirQ/NorQ/GpvN family protein (Roseobacter denitrificans OCh 114)</t>
+  </si>
+  <si>
+    <t>APZ15_RS35280</t>
+  </si>
+  <si>
+    <t>ATPase AAA (Burkholderia cepacia ATCC 25416)</t>
+  </si>
+  <si>
+    <t>PNI01S_RS24580</t>
+  </si>
+  <si>
+    <t>CbbQ/NirQ/NorQ/GpvN family protein (Pseudomonas nitroreducens NBRC 12694)</t>
+  </si>
+  <si>
+    <t>MAQ5080_RS04760</t>
+  </si>
+  <si>
+    <t>ATPase (Marinomonas aquimarina)</t>
+  </si>
+  <si>
+    <t>false_S</t>
   </si>
 </sst>
 </file>
@@ -827,11 +866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2787,6 +2826,180 @@
       </c>
       <c r="I67" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>140</v>
+      </c>
+      <c r="B68" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" t="s">
+        <v>152</v>
+      </c>
+      <c r="E68" t="s">
+        <v>152</v>
+      </c>
+      <c r="F68" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" t="s">
+        <v>32</v>
+      </c>
+      <c r="I68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E69" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" t="s">
+        <v>32</v>
+      </c>
+      <c r="I69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" t="s">
+        <v>144</v>
+      </c>
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+      <c r="E70" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" t="s">
+        <v>32</v>
+      </c>
+      <c r="I70" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>146</v>
+      </c>
+      <c r="B71" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" t="s">
+        <v>152</v>
+      </c>
+      <c r="E71" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" t="s">
+        <v>32</v>
+      </c>
+      <c r="I71" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>148</v>
+      </c>
+      <c r="B72" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" t="s">
+        <v>152</v>
+      </c>
+      <c r="E72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F72" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" t="s">
+        <v>32</v>
+      </c>
+      <c r="H72" t="s">
+        <v>32</v>
+      </c>
+      <c r="I72" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C73" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" t="s">
+        <v>152</v>
+      </c>
+      <c r="E73" t="s">
+        <v>152</v>
+      </c>
+      <c r="F73" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" t="s">
+        <v>32</v>
+      </c>
+      <c r="H73" t="s">
+        <v>32</v>
+      </c>
+      <c r="I73" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
False cobT/cobS genes are members of B12 pathway
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="156">
   <si>
     <t>_id</t>
   </si>
@@ -484,6 +484,15 @@
   </si>
   <si>
     <t>false_S</t>
+  </si>
+  <si>
+    <t>false_cobS</t>
+  </si>
+  <si>
+    <t>cobT_cobU</t>
+  </si>
+  <si>
+    <t>false_cobT</t>
   </si>
 </sst>
 </file>
@@ -869,8 +878,8 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="A1:I73"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,14 +2612,14 @@
       <c r="B60" t="s">
         <v>123</v>
       </c>
-      <c r="C60" t="s">
-        <v>32</v>
+      <c r="C60" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D60" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E60" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F60" t="s">
         <v>32</v>
@@ -2632,14 +2641,14 @@
       <c r="B61" t="s">
         <v>126</v>
       </c>
-      <c r="C61" t="s">
-        <v>32</v>
+      <c r="C61" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D61" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E61" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F61" t="s">
         <v>32</v>
@@ -2835,14 +2844,14 @@
       <c r="B68" t="s">
         <v>140</v>
       </c>
-      <c r="C68" t="s">
-        <v>32</v>
+      <c r="C68" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D68" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E68" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F68" t="s">
         <v>32</v>
@@ -2864,14 +2873,14 @@
       <c r="B69" t="s">
         <v>142</v>
       </c>
-      <c r="C69" t="s">
-        <v>32</v>
+      <c r="C69" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D69" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E69" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F69" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Better limits on the subunit lengths
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -879,7 +879,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,10 +943,10 @@
         <v>7</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="H2">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="I2" t="s">
         <v>32</v>
@@ -972,10 +972,10 @@
         <v>7</v>
       </c>
       <c r="G3">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="I3" t="s">
         <v>32</v>
@@ -1001,10 +1001,10 @@
         <v>7</v>
       </c>
       <c r="G4">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="H4">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
@@ -1030,10 +1030,10 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="H5">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="I5" t="s">
         <v>32</v>
@@ -1059,10 +1059,10 @@
         <v>15</v>
       </c>
       <c r="G6">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H6">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
@@ -1088,10 +1088,10 @@
         <v>15</v>
       </c>
       <c r="G7">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H7">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="I7" t="s">
         <v>32</v>
@@ -1117,10 +1117,10 @@
         <v>15</v>
       </c>
       <c r="G8">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H8">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
@@ -1146,10 +1146,10 @@
         <v>15</v>
       </c>
       <c r="G9">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="H9">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1175,10 +1175,10 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="H10">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I10" t="s">
         <v>32</v>
@@ -1204,10 +1204,10 @@
         <v>11</v>
       </c>
       <c r="G11">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="H11">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I11" t="s">
         <v>32</v>
@@ -1233,10 +1233,10 @@
         <v>11</v>
       </c>
       <c r="G12">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="H12">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I12" t="s">
         <v>32</v>
@@ -1262,10 +1262,10 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="H13">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="I13" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Putative Actinobacterial S-subunit was added
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="158">
   <si>
     <t>_id</t>
   </si>
@@ -493,6 +493,12 @@
   </si>
   <si>
     <t>false_cobT</t>
+  </si>
+  <si>
+    <t>WP_085243324.1</t>
+  </si>
+  <si>
+    <t>Putative S-subunit in Actinobacteria [Mycobacterium europaeum]</t>
   </si>
 </sst>
 </file>
@@ -875,11 +881,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11:H13"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1273,45 +1279,45 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>300</v>
+      </c>
+      <c r="H14">
+        <v>500</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>32</v>
@@ -1331,16 +1337,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
@@ -1360,19 +1366,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
         <v>32</v>
@@ -1389,19 +1395,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
@@ -1418,19 +1424,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
@@ -1447,19 +1453,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F20" t="s">
         <v>32</v>
@@ -1476,19 +1482,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -1505,19 +1511,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
         <v>32</v>
@@ -1534,19 +1540,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s">
         <v>32</v>
@@ -1563,19 +1569,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F24" t="s">
         <v>32</v>
@@ -1592,19 +1598,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
         <v>32</v>
@@ -1621,19 +1627,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="F26" t="s">
         <v>32</v>
@@ -1650,16 +1656,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
         <v>32</v>
@@ -1679,16 +1685,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -1708,16 +1714,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
         <v>32</v>
@@ -1737,16 +1743,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
         <v>32</v>
@@ -1766,16 +1772,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
         <v>32</v>
@@ -1795,16 +1801,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
         <v>32</v>
@@ -1824,16 +1830,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>
@@ -1853,19 +1859,19 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F34" t="s">
         <v>32</v>
@@ -1882,19 +1888,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F35" t="s">
         <v>32</v>
@@ -1911,19 +1917,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
+        <v>64</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F36" t="s">
         <v>32</v>
@@ -1940,19 +1946,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F37" t="s">
         <v>32</v>
@@ -1969,19 +1975,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F38" t="s">
         <v>32</v>
@@ -1998,19 +2004,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F39" t="s">
         <v>32</v>
@@ -2027,19 +2033,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F40" t="s">
         <v>32</v>
@@ -2056,19 +2062,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F41" t="s">
         <v>32</v>
@@ -2085,16 +2091,16 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
         <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
         <v>32</v>
@@ -2114,19 +2120,19 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F43" t="s">
         <v>32</v>
@@ -2143,19 +2149,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
         <v>32</v>
@@ -2172,16 +2178,16 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E45" t="s">
         <v>32</v>
@@ -2201,16 +2207,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E46" t="s">
         <v>32</v>
@@ -2230,10 +2236,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
@@ -2259,16 +2265,16 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
         <v>32</v>
@@ -2288,16 +2294,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
         <v>32</v>
@@ -2317,16 +2323,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
@@ -2346,19 +2352,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F51" t="s">
         <v>32</v>
@@ -2375,19 +2381,19 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="E52" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F52" t="s">
         <v>32</v>
@@ -2404,16 +2410,16 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
         <v>32</v>
@@ -2433,16 +2439,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
         <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E54" t="s">
         <v>32</v>
@@ -2462,19 +2468,19 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
         <v>19</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="E55" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F55" t="s">
         <v>32</v>
@@ -2491,19 +2497,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C56" t="s">
         <v>19</v>
       </c>
       <c r="D56" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="E56" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F56" t="s">
         <v>32</v>
@@ -2520,16 +2526,16 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
       </c>
       <c r="D57" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E57" t="s">
         <v>32</v>
@@ -2549,16 +2555,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B58" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C58" t="s">
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E58" t="s">
         <v>32</v>
@@ -2578,16 +2584,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E59" t="s">
         <v>32</v>
@@ -2607,19 +2613,19 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>47</v>
+        <v>103</v>
+      </c>
+      <c r="C60" t="s">
+        <v>19</v>
       </c>
       <c r="D60" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="E60" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="F60" t="s">
         <v>32</v>
@@ -2631,15 +2637,15 @@
         <v>32</v>
       </c>
       <c r="I60" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>47</v>
@@ -2660,24 +2666,24 @@
         <v>32</v>
       </c>
       <c r="I61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
-      </c>
-      <c r="C62" t="s">
-        <v>32</v>
+        <v>126</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D62" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E62" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F62" t="s">
         <v>32</v>
@@ -2689,15 +2695,15 @@
         <v>32</v>
       </c>
       <c r="I62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C63" t="s">
         <v>32</v>
@@ -2718,15 +2724,15 @@
         <v>32</v>
       </c>
       <c r="I63" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
@@ -2747,15 +2753,15 @@
         <v>32</v>
       </c>
       <c r="I64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C65" t="s">
         <v>32</v>
@@ -2776,15 +2782,15 @@
         <v>32</v>
       </c>
       <c r="I65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C66" t="s">
         <v>32</v>
@@ -2805,15 +2811,15 @@
         <v>32</v>
       </c>
       <c r="I66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
         <v>32</v>
@@ -2834,24 +2840,24 @@
         <v>32</v>
       </c>
       <c r="I67" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>47</v>
+        <v>138</v>
+      </c>
+      <c r="C68" t="s">
+        <v>32</v>
       </c>
       <c r="D68" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="F68" t="s">
         <v>32</v>
@@ -2863,15 +2869,15 @@
         <v>32</v>
       </c>
       <c r="I68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>47</v>
@@ -2892,24 +2898,24 @@
         <v>32</v>
       </c>
       <c r="I69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
-      </c>
-      <c r="C70" t="s">
-        <v>32</v>
+        <v>142</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D70" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E70" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F70" t="s">
         <v>32</v>
@@ -2921,15 +2927,15 @@
         <v>32</v>
       </c>
       <c r="I70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71" t="s">
         <v>32</v>
@@ -2950,15 +2956,15 @@
         <v>32</v>
       </c>
       <c r="I71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C72" t="s">
         <v>32</v>
@@ -2979,15 +2985,15 @@
         <v>32</v>
       </c>
       <c r="I72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C73" t="s">
         <v>32</v>
@@ -3008,6 +3014,35 @@
         <v>32</v>
       </c>
       <c r="I73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B74" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74" t="s">
+        <v>152</v>
+      </c>
+      <c r="E74" t="s">
+        <v>152</v>
+      </c>
+      <c r="F74" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Some length thresholds were changed back to the old values
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -885,7 +885,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -949,10 +949,10 @@
         <v>7</v>
       </c>
       <c r="G2">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="H2">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I2" t="s">
         <v>32</v>
@@ -978,10 +978,10 @@
         <v>7</v>
       </c>
       <c r="G3">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="H3">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I3" t="s">
         <v>32</v>
@@ -1007,10 +1007,10 @@
         <v>7</v>
       </c>
       <c r="G4">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="H4">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I4" t="s">
         <v>32</v>
@@ -1036,10 +1036,10 @@
         <v>7</v>
       </c>
       <c r="G5">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="H5">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I5" t="s">
         <v>32</v>
@@ -1068,7 +1068,7 @@
         <v>500</v>
       </c>
       <c r="H6">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="I6" t="s">
         <v>32</v>
@@ -1097,7 +1097,7 @@
         <v>500</v>
       </c>
       <c r="H7">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="I7" t="s">
         <v>32</v>
@@ -1126,7 +1126,7 @@
         <v>500</v>
       </c>
       <c r="H8">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="I8" t="s">
         <v>32</v>
@@ -1155,7 +1155,7 @@
         <v>500</v>
       </c>
       <c r="H9">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1181,7 +1181,7 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H10">
         <v>500</v>
@@ -1210,7 +1210,7 @@
         <v>11</v>
       </c>
       <c r="G11">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H11">
         <v>500</v>
@@ -1239,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="G12">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H12">
         <v>500</v>
@@ -1268,7 +1268,7 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H13">
         <v>500</v>
@@ -1297,7 +1297,7 @@
         <v>11</v>
       </c>
       <c r="G14">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="H14">
         <v>500</v>

</xml_diff>

<commit_message>
MoxR family ATPase is now considered as small chelatase subunit
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="160">
   <si>
     <t>_id</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t>Putative S-subunit in Actinobacteria [Mycobacterium europaeum]</t>
+  </si>
+  <si>
+    <t>Putative S-subunit in Archaea (MoxR family ATPase) [PMID: 22491058, 21148420]</t>
+  </si>
+  <si>
+    <t>WP_006076756.1</t>
   </si>
 </sst>
 </file>
@@ -881,11 +887,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,45 +1314,45 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>250</v>
+      </c>
+      <c r="H15">
+        <v>500</v>
       </c>
       <c r="I15" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
@@ -1366,16 +1372,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -1395,19 +1401,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
         <v>32</v>
@@ -1424,19 +1430,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
         <v>32</v>
@@ -1453,19 +1459,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
         <v>32</v>
@@ -1482,19 +1488,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
         <v>32</v>
@@ -1511,19 +1517,19 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
         <v>32</v>
@@ -1540,19 +1546,19 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F23" t="s">
         <v>32</v>
@@ -1569,19 +1575,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s">
         <v>32</v>
@@ -1598,19 +1604,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
         <v>32</v>
@@ -1627,19 +1633,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F26" t="s">
         <v>32</v>
@@ -1656,19 +1662,19 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
         <v>32</v>
@@ -1685,16 +1691,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>32</v>
@@ -1714,16 +1720,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>32</v>
@@ -1743,16 +1749,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
         <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
         <v>32</v>
@@ -1772,16 +1778,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
         <v>32</v>
@@ -1801,16 +1807,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
         <v>32</v>
@@ -1830,16 +1836,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>
@@ -1859,16 +1865,16 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
         <v>32</v>
@@ -1888,19 +1894,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F35" t="s">
         <v>32</v>
@@ -1917,19 +1923,19 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F36" t="s">
         <v>32</v>
@@ -1946,19 +1952,19 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>19</v>
+        <v>64</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
         <v>32</v>
@@ -1975,19 +1981,19 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F38" t="s">
         <v>32</v>
@@ -2004,19 +2010,19 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F39" t="s">
         <v>32</v>
@@ -2033,19 +2039,19 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F40" t="s">
         <v>32</v>
@@ -2062,19 +2068,19 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="F41" t="s">
         <v>32</v>
@@ -2091,19 +2097,19 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="C42" t="s">
         <v>19</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F42" t="s">
         <v>32</v>
@@ -2120,16 +2126,16 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
         <v>19</v>
       </c>
       <c r="D43" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="E43" t="s">
         <v>32</v>
@@ -2149,19 +2155,19 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E44" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F44" t="s">
         <v>32</v>
@@ -2178,19 +2184,19 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F45" t="s">
         <v>32</v>
@@ -2207,16 +2213,16 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C46" t="s">
         <v>19</v>
       </c>
       <c r="D46" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E46" t="s">
         <v>32</v>
@@ -2236,16 +2242,16 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
         <v>19</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E47" t="s">
         <v>32</v>
@@ -2265,10 +2271,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
@@ -2294,16 +2300,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
         <v>19</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E49" t="s">
         <v>32</v>
@@ -2323,16 +2329,16 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E50" t="s">
         <v>32</v>
@@ -2352,16 +2358,16 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
         <v>19</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E51" t="s">
         <v>32</v>
@@ -2381,19 +2387,19 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="E52" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F52" t="s">
         <v>32</v>
@@ -2410,19 +2416,19 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C53" t="s">
         <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="E53" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F53" t="s">
         <v>32</v>
@@ -2439,16 +2445,16 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C54" t="s">
         <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E54" t="s">
         <v>32</v>
@@ -2468,16 +2474,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
         <v>19</v>
       </c>
       <c r="D55" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E55" t="s">
         <v>32</v>
@@ -2497,19 +2503,19 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
         <v>19</v>
       </c>
       <c r="D56" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="E56" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F56" t="s">
         <v>32</v>
@@ -2526,19 +2532,19 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
       </c>
       <c r="D57" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="E57" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F57" t="s">
         <v>32</v>
@@ -2555,16 +2561,16 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E58" t="s">
         <v>32</v>
@@ -2584,16 +2590,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E59" t="s">
         <v>32</v>
@@ -2613,16 +2619,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C60" t="s">
         <v>19</v>
       </c>
       <c r="D60" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E60" t="s">
         <v>32</v>
@@ -2642,19 +2648,19 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>47</v>
+        <v>103</v>
+      </c>
+      <c r="C61" t="s">
+        <v>19</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="E61" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="F61" t="s">
         <v>32</v>
@@ -2666,15 +2672,15 @@
         <v>32</v>
       </c>
       <c r="I61" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>47</v>
@@ -2695,24 +2701,24 @@
         <v>32</v>
       </c>
       <c r="I62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
-      </c>
-      <c r="C63" t="s">
-        <v>32</v>
+        <v>126</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D63" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
       <c r="F63" t="s">
         <v>32</v>
@@ -2724,15 +2730,15 @@
         <v>32</v>
       </c>
       <c r="I63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
@@ -2753,15 +2759,15 @@
         <v>32</v>
       </c>
       <c r="I64" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
         <v>32</v>
@@ -2782,15 +2788,15 @@
         <v>32</v>
       </c>
       <c r="I65" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66" t="s">
         <v>32</v>
@@ -2811,15 +2817,15 @@
         <v>32</v>
       </c>
       <c r="I66" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
         <v>32</v>
@@ -2840,15 +2846,15 @@
         <v>32</v>
       </c>
       <c r="I67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C68" t="s">
         <v>32</v>
@@ -2869,24 +2875,24 @@
         <v>32</v>
       </c>
       <c r="I68" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B69" t="s">
-        <v>140</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>47</v>
+        <v>138</v>
+      </c>
+      <c r="C69" t="s">
+        <v>32</v>
       </c>
       <c r="D69" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="E69" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="F69" t="s">
         <v>32</v>
@@ -2898,15 +2904,15 @@
         <v>32</v>
       </c>
       <c r="I69" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>47</v>
@@ -2927,24 +2933,24 @@
         <v>32</v>
       </c>
       <c r="I70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
-      </c>
-      <c r="C71" t="s">
-        <v>32</v>
+        <v>142</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D71" t="s">
-        <v>152</v>
+        <v>78</v>
       </c>
       <c r="E71" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F71" t="s">
         <v>32</v>
@@ -2956,15 +2962,15 @@
         <v>32</v>
       </c>
       <c r="I71" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
         <v>32</v>
@@ -2985,15 +2991,15 @@
         <v>32</v>
       </c>
       <c r="I72" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C73" t="s">
         <v>32</v>
@@ -3014,15 +3020,15 @@
         <v>32</v>
       </c>
       <c r="I73" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C74" t="s">
         <v>32</v>
@@ -3043,6 +3049,35 @@
         <v>32</v>
       </c>
       <c r="I74" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>150</v>
+      </c>
+      <c r="B75" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" t="s">
+        <v>32</v>
+      </c>
+      <c r="D75" t="s">
+        <v>152</v>
+      </c>
+      <c r="E75" t="s">
+        <v>152</v>
+      </c>
+      <c r="F75" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" t="s">
         <v>151</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moxR is not considered as a small chelatase subunit anymore..
</commit_message>
<xml_diff>
--- a/chelatase_db/data/pathway_genes.xlsx
+++ b/chelatase_db/data/pathway_genes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="161">
   <si>
     <t>_id</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>WP_006076756.1</t>
+  </si>
+  <si>
+    <t>MoxR</t>
   </si>
 </sst>
 </file>
@@ -890,8 +893,8 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,16 +1323,16 @@
         <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G15">
         <v>250</v>

</xml_diff>